<commit_message>
Cleaning up experimental datasheet
</commit_message>
<xml_diff>
--- a/tests/tropic/input_experimental.xlsx
+++ b/tests/tropic/input_experimental.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Arch\home\rmrr\larest\larest-main\tests\tropic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CDE2C6-AFA4-4407-8F40-3E3ADB50A42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457BBD31-0986-4F40-B2E1-70C9C8069AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1450" yWindow="-19520" windowWidth="28800" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="318">
   <si>
     <t>monomer_smiles</t>
   </si>
@@ -849,18 +849,6 @@
     <t>O=C2Cc1ccccc1CCO2</t>
   </si>
   <si>
-    <t>toluene_d9</t>
-  </si>
-  <si>
-    <t>toluene_d10</t>
-  </si>
-  <si>
-    <t>toluene_d11</t>
-  </si>
-  <si>
-    <t>toluene_d12</t>
-  </si>
-  <si>
     <t>Cai_Zhu_2023_NatCommun_M1</t>
   </si>
   <si>
@@ -1006,9 +994,6 @@
   </si>
   <si>
     <t>duplicate</t>
-  </si>
-  <si>
-    <t>values from review (duplicate)</t>
   </si>
 </sst>
 </file>
@@ -1505,10 +1490,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AL171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="39" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="AD100" sqref="AD100"/>
+      <selection pane="bottomLeft" activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1607,19 +1592,19 @@
         <v>9</v>
       </c>
       <c r="R1" s="13" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="S1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="T1" s="13" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="U1" s="11" t="s">
         <v>97</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="W1" s="11" t="s">
         <v>25</v>
@@ -1646,7 +1631,7 @@
         <v>22</v>
       </c>
       <c r="AE1" s="11" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="AF1" s="11" t="s">
         <v>117</v>
@@ -1913,7 +1898,7 @@
         <v>62</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1973,7 +1958,7 @@
         <v>62</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>66</v>
@@ -2016,7 +2001,7 @@
         <v>62</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>64</v>
@@ -2059,7 +2044,7 @@
         <v>62</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>66</v>
@@ -2102,7 +2087,7 @@
         <v>62</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="Q10" s="4">
         <v>0.4</v>
@@ -2122,41 +2107,47 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:38" s="29" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
+      <c r="B11" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="1" t="s">
+      <c r="K11" s="31"/>
+      <c r="L11" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="32">
         <v>5.0999999999999996</v>
       </c>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4">
+      <c r="R11" s="32"/>
+      <c r="S11" s="32">
         <v>-29.9</v>
       </c>
-      <c r="T11" s="4"/>
-      <c r="X11" s="3" t="s">
+      <c r="T11" s="32"/>
+      <c r="W11" s="29">
+        <v>2009</v>
+      </c>
+      <c r="X11" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="AD11" s="1" t="s">
-        <v>322</v>
+      <c r="AD11" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE11" s="29" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:38" s="29" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2179,7 +2170,7 @@
         <v>62</v>
       </c>
       <c r="M12" s="29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="Q12" s="32">
         <v>-82.3</v>
@@ -2189,11 +2180,17 @@
         <v>-74</v>
       </c>
       <c r="T12" s="32"/>
+      <c r="W12" s="29">
+        <v>2009</v>
+      </c>
       <c r="X12" s="31" t="s">
         <v>74</v>
       </c>
       <c r="AD12" s="29" t="s">
-        <v>322</v>
+        <v>131</v>
+      </c>
+      <c r="AE12" s="29" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2616,7 +2613,7 @@
         <v>62</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N22" s="1">
         <v>298</v>
@@ -2656,7 +2653,7 @@
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>158</v>
@@ -2699,7 +2696,7 @@
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>158</v>
@@ -2742,7 +2739,7 @@
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>63</v>
@@ -2788,7 +2785,7 @@
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>63</v>
@@ -2832,7 +2829,7 @@
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>63</v>
@@ -2873,10 +2870,10 @@
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N28" s="1">
         <v>298</v>
@@ -4831,11 +4828,14 @@
       <c r="T67" s="32">
         <v>2</v>
       </c>
+      <c r="W67" s="29">
+        <v>2025</v>
+      </c>
       <c r="X67" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="AD67" s="29" t="s">
-        <v>321</v>
+      <c r="AE67" s="29" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="68" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -6402,10 +6402,10 @@
       </c>
       <c r="K100" s="3"/>
       <c r="L100" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N100" s="1">
         <v>298.14999999999998</v>
@@ -6448,7 +6448,7 @@
         <v>62</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N101" s="1">
         <v>298.14999999999998</v>
@@ -6491,7 +6491,7 @@
         <v>62</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N102" s="1">
         <v>298.14999999999998</v>
@@ -6531,10 +6531,10 @@
       </c>
       <c r="K103" s="31"/>
       <c r="L103" s="29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M103" s="29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N103" s="29">
         <v>298.14999999999998</v>
@@ -6550,11 +6550,14 @@
         <v>-86</v>
       </c>
       <c r="T103" s="32"/>
+      <c r="W103" s="29">
+        <v>1996</v>
+      </c>
       <c r="X103" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="AD103" s="29" t="s">
-        <v>321</v>
+      <c r="AE103" s="29" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="104" spans="1:38" s="29" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -6574,7 +6577,7 @@
       </c>
       <c r="K104" s="31"/>
       <c r="L104" s="29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M104" s="29" t="s">
         <v>63</v>
@@ -6593,11 +6596,14 @@
         <v>41</v>
       </c>
       <c r="T104" s="32"/>
+      <c r="W104" s="29">
+        <v>1996</v>
+      </c>
       <c r="X104" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="AD104" s="29" t="s">
-        <v>321</v>
+      <c r="AE104" s="29" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="105" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -6620,7 +6626,7 @@
         <v>62</v>
       </c>
       <c r="M105" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N105" s="1">
         <v>298.14999999999998</v>
@@ -6706,7 +6712,7 @@
         <v>62</v>
       </c>
       <c r="M107" s="29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N107" s="29">
         <v>298.14999999999998</v>
@@ -6722,11 +6728,14 @@
         <v>-74</v>
       </c>
       <c r="T107" s="32"/>
+      <c r="W107" s="29">
+        <v>1996</v>
+      </c>
       <c r="X107" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="AD107" s="29" t="s">
-        <v>321</v>
+      <c r="AE107" s="29" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="108" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -6749,7 +6758,7 @@
         <v>62</v>
       </c>
       <c r="M108" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N108" s="1">
         <v>298.14999999999998</v>
@@ -6878,7 +6887,7 @@
         <v>62</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N111" s="1">
         <v>298.14999999999998</v>
@@ -6964,7 +6973,7 @@
         <v>62</v>
       </c>
       <c r="M113" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N113" s="1">
         <v>298.14999999999998</v>
@@ -7050,7 +7059,7 @@
         <v>62</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N115" s="1">
         <v>298.14999999999998</v>
@@ -7133,10 +7142,10 @@
       </c>
       <c r="K117" s="3"/>
       <c r="L117" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N117" s="1">
         <v>298.14999999999998</v>
@@ -7176,7 +7185,7 @@
       </c>
       <c r="K118" s="3"/>
       <c r="L118" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M118" s="1" t="s">
         <v>63</v>
@@ -8156,7 +8165,7 @@
         <v>2024</v>
       </c>
       <c r="X139" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="AF139" s="1" t="s">
         <v>253</v>
@@ -8203,44 +8212,44 @@
         <v>2024</v>
       </c>
       <c r="X140" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="AF140" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="141" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141" s="1" t="s">
+    <row r="141" spans="1:32" s="29" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C141" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K141" s="3"/>
-      <c r="P141" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q141" s="4">
+      <c r="B141" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C141" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K141" s="31"/>
+      <c r="P141" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q141" s="32">
         <v>-9.4</v>
       </c>
-      <c r="R141" s="4"/>
-      <c r="S141" s="4">
+      <c r="R141" s="32"/>
+      <c r="S141" s="32">
         <v>-28.1</v>
       </c>
-      <c r="T141" s="4"/>
-      <c r="W141" s="1">
+      <c r="T141" s="32"/>
+      <c r="W141" s="29">
         <v>2020</v>
       </c>
-      <c r="X141" s="1" t="s">
+      <c r="X141" s="29" t="s">
         <v>247</v>
       </c>
-      <c r="AD141" s="1" t="s">
+      <c r="AD141" s="29" t="s">
         <v>257</v>
       </c>
-      <c r="AE141" s="1" t="s">
+      <c r="AE141" s="29" t="s">
         <v>258</v>
       </c>
     </row>
@@ -8388,7 +8397,7 @@
         <v>255</v>
       </c>
       <c r="AF144" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="145" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8439,7 +8448,7 @@
         <v>255</v>
       </c>
       <c r="AF145" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="146" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8490,7 +8499,7 @@
         <v>255</v>
       </c>
       <c r="AF146" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="147" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8541,7 +8550,7 @@
         <v>255</v>
       </c>
       <c r="AF147" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="148" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8592,7 +8601,7 @@
         <v>255</v>
       </c>
       <c r="AF148" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="149" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8643,7 +8652,7 @@
         <v>255</v>
       </c>
       <c r="AF149" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="150" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8694,12 +8703,12 @@
         <v>255</v>
       </c>
       <c r="AF150" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="151" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>59</v>
@@ -8714,7 +8723,7 @@
         <v>4</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>269</v>
+        <v>177</v>
       </c>
       <c r="K151" s="3"/>
       <c r="L151" s="1" t="s">
@@ -8741,12 +8750,12 @@
         <v>255</v>
       </c>
       <c r="AF151" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="152" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>59</v>
@@ -8761,7 +8770,7 @@
         <v>4</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>270</v>
+        <v>177</v>
       </c>
       <c r="K152" s="3"/>
       <c r="L152" s="1" t="s">
@@ -8788,12 +8797,12 @@
         <v>255</v>
       </c>
       <c r="AF152" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="153" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>59</v>
@@ -8808,7 +8817,7 @@
         <v>4</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>271</v>
+        <v>177</v>
       </c>
       <c r="K153" s="3"/>
       <c r="L153" s="1" t="s">
@@ -8835,12 +8844,12 @@
         <v>255</v>
       </c>
       <c r="AF153" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="154" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>59</v>
@@ -8855,7 +8864,7 @@
         <v>4</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>272</v>
+        <v>177</v>
       </c>
       <c r="K154" s="3"/>
       <c r="L154" s="1" t="s">
@@ -8882,12 +8891,12 @@
         <v>255</v>
       </c>
       <c r="AF154" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="155" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>59</v>
@@ -8920,15 +8929,15 @@
         <v>2010</v>
       </c>
       <c r="X155" s="17" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="AF155" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="156" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>59</v>
@@ -8971,12 +8980,12 @@
         <v>2017</v>
       </c>
       <c r="X156" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="157" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>59</v>
@@ -9009,12 +9018,12 @@
         <v>2014</v>
       </c>
       <c r="X157" s="17" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="158" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>98</v>
@@ -9058,12 +9067,12 @@
         <v>2014</v>
       </c>
       <c r="X158" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="159" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>98</v>
@@ -9107,12 +9116,12 @@
         <v>2014</v>
       </c>
       <c r="X159" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="160" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>59</v>
@@ -9151,7 +9160,7 @@
         <v>2014</v>
       </c>
       <c r="X160" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="161" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9202,10 +9211,10 @@
         <v>2025</v>
       </c>
       <c r="X161" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="AF161" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="162" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9256,10 +9265,10 @@
         <v>2025</v>
       </c>
       <c r="X162" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AF162" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="AF162" s="1" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="163" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9310,10 +9319,10 @@
         <v>2025</v>
       </c>
       <c r="X163" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="AF163" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="164" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9364,10 +9373,10 @@
         <v>2025</v>
       </c>
       <c r="X164" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="AF164" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="165" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9411,7 +9420,7 @@
         <v>2024</v>
       </c>
       <c r="X165" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="166" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9455,22 +9464,22 @@
         <v>2024</v>
       </c>
       <c r="X166" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y166" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z166" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AA166" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="AB166" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="Y166" s="1" t="s">
+      <c r="AC166" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="Z166" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="AA166" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="AB166" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="AC166" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="167" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9514,7 +9523,7 @@
         <v>2024</v>
       </c>
       <c r="X167" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="168" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9558,7 +9567,7 @@
         <v>2024</v>
       </c>
       <c r="X168" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="169" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9602,7 +9611,7 @@
         <v>2024</v>
       </c>
       <c r="X169" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="170" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9646,7 +9655,7 @@
         <v>2024</v>
       </c>
       <c r="X170" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="171" spans="1:32" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -9690,7 +9699,7 @@
         <v>2024</v>
       </c>
       <c r="X171" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -9717,7 +9726,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C2">
         <v>8.3140000000000001</v>
@@ -9725,7 +9734,7 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="22" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C3" s="23">
         <v>4.1840000000000002</v>
@@ -9743,7 +9752,7 @@
       <c r="B5" s="22"/>
       <c r="C5" s="23"/>
       <c r="E5" s="22" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F5" s="23">
         <v>-2.3610000000000002</v>
@@ -9757,7 +9766,7 @@
       <c r="B6" s="22"/>
       <c r="C6" s="23"/>
       <c r="E6" s="22" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F6" s="23">
         <v>-6.1356999999999999</v>
@@ -9779,6 +9788,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="240bb28e-6377-48b0-832f-151ffa71870e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5f270ae-dbad-4cfd-80e2-71659db687aa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002914CBC9445B8347939C6B4510D67668" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="debcf52f3d4c81bc84586c816ca1bc65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5f270ae-dbad-4cfd-80e2-71659db687aa" xmlns:ns3="240bb28e-6377-48b0-832f-151ffa71870e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0db2ad47acd613f43945cc47365a45bf" ns2:_="" ns3:_="">
     <xsd:import namespace="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
@@ -10007,41 +10036,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="240bb28e-6377-48b0-832f-151ffa71870e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5f270ae-dbad-4cfd-80e2-71659db687aa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62789F9-1650-4133-931E-1E27A89DED57}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31F8A5B-9EBA-4355-A82B-5141D4A521CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
-    <ds:schemaRef ds:uri="240bb28e-6377-48b0-832f-151ffa71870e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10064,9 +10062,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31F8A5B-9EBA-4355-A82B-5141D4A521CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62789F9-1650-4133-931E-1E27A89DED57}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
+    <ds:schemaRef ds:uri="240bb28e-6377-48b0-832f-151ffa71870e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to tropic dataset run
</commit_message>
<xml_diff>
--- a/tests/tropic/input_experimental.xlsx
+++ b/tests/tropic/input_experimental.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Arch\home\rmrr\larest\larest-main\tests\tropic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Arch\home\rmrr\larest\larest-dev\tests\tropic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457BBD31-0986-4F40-B2E1-70C9C8069AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B48318B-1376-47FF-9694-699998185867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1450" yWindow="-19520" windowWidth="28800" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2010" yWindow="-18960" windowWidth="28800" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -1490,10 +1490,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AL171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="B142" sqref="B142"/>
+      <selection pane="bottomLeft" activeCell="F161" sqref="F161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -9788,26 +9788,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="240bb28e-6377-48b0-832f-151ffa71870e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5f270ae-dbad-4cfd-80e2-71659db687aa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002914CBC9445B8347939C6B4510D67668" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="debcf52f3d4c81bc84586c816ca1bc65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5f270ae-dbad-4cfd-80e2-71659db687aa" xmlns:ns3="240bb28e-6377-48b0-832f-151ffa71870e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0db2ad47acd613f43945cc47365a45bf" ns2:_="" ns3:_="">
     <xsd:import namespace="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
@@ -10036,10 +10016,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="240bb28e-6377-48b0-832f-151ffa71870e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5f270ae-dbad-4cfd-80e2-71659db687aa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31F8A5B-9EBA-4355-A82B-5141D4A521CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62789F9-1650-4133-931E-1E27A89DED57}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
+    <ds:schemaRef ds:uri="240bb28e-6377-48b0-832f-151ffa71870e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10062,20 +10073,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62789F9-1650-4133-931E-1E27A89DED57}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31F8A5B-9EBA-4355-A82B-5141D4A521CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
-    <ds:schemaRef ds:uri="240bb28e-6377-48b0-832f-151ffa71870e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to configs and plotting functions for tropic and ring size
</commit_message>
<xml_diff>
--- a/tests/tropic/input_experimental.xlsx
+++ b/tests/tropic/input_experimental.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Arch\home\rmrr\larest\larest-dev\tests\tropic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B48318B-1376-47FF-9694-699998185867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBC4D4D-E012-4C50-90B1-D570FAD2FB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="-18960" windowWidth="28800" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="654" yWindow="438" windowWidth="19110" windowHeight="11346" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="318">
   <si>
     <t>monomer_smiles</t>
   </si>
@@ -1490,10 +1490,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AL171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="F161" sqref="F161"/>
+      <selection pane="bottomLeft" activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1701,7 +1701,9 @@
       <c r="W2" s="1">
         <v>2002</v>
       </c>
-      <c r="X2" s="3"/>
+      <c r="X2" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="AF2" s="1" t="s">
         <v>123</v>
       </c>
@@ -9788,6 +9790,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="240bb28e-6377-48b0-832f-151ffa71870e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5f270ae-dbad-4cfd-80e2-71659db687aa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002914CBC9445B8347939C6B4510D67668" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="debcf52f3d4c81bc84586c816ca1bc65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5f270ae-dbad-4cfd-80e2-71659db687aa" xmlns:ns3="240bb28e-6377-48b0-832f-151ffa71870e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0db2ad47acd613f43945cc47365a45bf" ns2:_="" ns3:_="">
     <xsd:import namespace="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
@@ -10016,41 +10038,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="240bb28e-6377-48b0-832f-151ffa71870e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5f270ae-dbad-4cfd-80e2-71659db687aa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62789F9-1650-4133-931E-1E27A89DED57}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31F8A5B-9EBA-4355-A82B-5141D4A521CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
-    <ds:schemaRef ds:uri="240bb28e-6377-48b0-832f-151ffa71870e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10073,9 +10064,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E31F8A5B-9EBA-4355-A82B-5141D4A521CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62789F9-1650-4133-931E-1E27A89DED57}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5f270ae-dbad-4cfd-80e2-71659db687aa"/>
+    <ds:schemaRef ds:uri="240bb28e-6377-48b0-832f-151ffa71870e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>